<commit_message>
Got the timing stuff working, and I was able to redo the basic tests for neuron counts ranging from 2^10-2^24 th. Awesome results.
</commit_message>
<xml_diff>
--- a/Libraries/OpenNeuronCL/PerformanceStats.xlsx
+++ b/Libraries/OpenNeuronCL/PerformanceStats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="1305" windowWidth="11010" windowHeight="11790"/>
+    <workbookView xWindow="4560" yWindow="1305" windowWidth="11010" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="FastSpiking Phase 1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Time</t>
   </si>
@@ -30,31 +30,7 @@
     <t>Error</t>
   </si>
   <si>
-    <t>OCL 100_100</t>
-  </si>
-  <si>
-    <t>OCL256_256</t>
-  </si>
-  <si>
-    <t>OCL512_512</t>
-  </si>
-  <si>
-    <t>OCL_1024_512</t>
-  </si>
-  <si>
     <t>OCL_Neurons_WorkItems</t>
-  </si>
-  <si>
-    <t>OCL_2048_512</t>
-  </si>
-  <si>
-    <t>OCL_4096_512</t>
-  </si>
-  <si>
-    <t>OCL_8192_256</t>
-  </si>
-  <si>
-    <t>OCL_16384_512</t>
   </si>
   <si>
     <t>Average</t>
@@ -73,6 +49,36 @@
   </si>
   <si>
     <t>% Increase</t>
+  </si>
+  <si>
+    <t>Neural Step</t>
+  </si>
+  <si>
+    <t>Sim time</t>
+  </si>
+  <si>
+    <t>OCL 2^10</t>
+  </si>
+  <si>
+    <t>OCL 2^12</t>
+  </si>
+  <si>
+    <t>OCL 2^14</t>
+  </si>
+  <si>
+    <t>OCL 2^16</t>
+  </si>
+  <si>
+    <t>OCL 2^18</t>
+  </si>
+  <si>
+    <t>OCL 2^20</t>
+  </si>
+  <si>
+    <t>OCL 2^23</t>
+  </si>
+  <si>
+    <t>OCL 2^24</t>
   </si>
 </sst>
 </file>
@@ -108,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12226,11 +12233,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="102576896"/>
-        <c:axId val="102578432"/>
+        <c:axId val="100680448"/>
+        <c:axId val="100681984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102576896"/>
+        <c:axId val="100680448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12240,12 +12247,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102578432"/>
+        <c:crossAx val="100681984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102578432"/>
+        <c:axId val="100681984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12256,7 +12263,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102576896"/>
+        <c:crossAx val="100680448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12309,10 +12316,10 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'FastSpiking Phase 1'!$X$14:$AG$14</c:f>
+                <c:f>'FastSpiking Phase 1'!$X$14:$AF$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
+                  <c:ptCount val="9"/>
                   <c:pt idx="0">
                     <c:v>9.9474631418057582E-3</c:v>
                   </c:pt>
@@ -12320,38 +12327,35 @@
                     <c:v>8.5449813137914027E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.7847424542773674E-3</c:v>
+                    <c:v>8.6579300205072126E-4</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9851950584514359E-3</c:v>
+                    <c:v>2.6587871803512206E-3</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.9185689120012222E-3</c:v>
+                    <c:v>3.4761464345450122E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.513451159568752E-3</c:v>
+                    <c:v>2.1269042504071501E-3</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>7.7375000000000013E-4</c:v>
+                    <c:v>1.9088539550211792E-3</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>2.9136938122233933E-3</c:v>
+                    <c:v>1.7411217193522112E-3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>1.5406196463508507E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>3.7964362089845378E-3</c:v>
+                    <c:v>1.2135725056213161E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'FastSpiking Phase 1'!$X$14:$AG$14</c:f>
+                <c:f>'FastSpiking Phase 1'!$X$14:$AF$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
+                  <c:ptCount val="9"/>
                   <c:pt idx="0">
                     <c:v>9.9474631418057582E-3</c:v>
                   </c:pt>
@@ -12359,28 +12363,25 @@
                     <c:v>8.5449813137914027E-3</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.7847424542773674E-3</c:v>
+                    <c:v>8.6579300205072126E-4</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.9851950584514359E-3</c:v>
+                    <c:v>2.6587871803512206E-3</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.9185689120012222E-3</c:v>
+                    <c:v>3.4761464345450122E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>1.513451159568752E-3</c:v>
+                    <c:v>2.1269042504071501E-3</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>7.7375000000000013E-4</c:v>
+                    <c:v>1.9088539550211792E-3</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>2.9136938122233933E-3</c:v>
+                    <c:v>1.7411217193522112E-3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>1.5406196463508507E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>3.7964362089845378E-3</c:v>
+                    <c:v>1.2135725056213161E-3</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -12398,38 +12399,38 @@
                   <c:v>FSP_100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>OCL 100_100</c:v>
+                  <c:v>OCL 2^10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>OCL256_256</c:v>
+                  <c:v>OCL 2^12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>OCL512_512</c:v>
+                  <c:v>OCL 2^14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>OCL_1024_512</c:v>
+                  <c:v>OCL 2^16</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>OCL_2048_512</c:v>
+                  <c:v>OCL 2^18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>OCL_4096_512</c:v>
+                  <c:v>OCL 2^20</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>OCL_8192_256</c:v>
+                  <c:v>OCL 2^23</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>OCL_16384_512</c:v>
+                  <c:v>OCL 2^24</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'FastSpiking Phase 1'!$X$13:$AG$13</c:f>
+              <c:f>'FastSpiking Phase 1'!$X$13:$AF$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>6.736370500000001E-2</c:v>
                 </c:pt>
@@ -12437,28 +12438,25 @@
                   <c:v>3.5546943999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.760663E-2</c:v>
+                  <c:v>2.7003640000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7827330000000001E-2</c:v>
+                  <c:v>2.8325259999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7897570000000003E-2</c:v>
+                  <c:v>2.951376E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6445139999999999E-2</c:v>
+                  <c:v>2.4075759999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.822305E-2</c:v>
+                  <c:v>2.597932E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.7555716666666664E-2</c:v>
+                  <c:v>2.3150120000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7690983333333332E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.6151533333333334E-2</c:v>
+                  <c:v>3.3666739999999994E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12473,11 +12471,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="102623488"/>
-        <c:axId val="102629760"/>
+        <c:axId val="100722944"/>
+        <c:axId val="100729216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102623488"/>
+        <c:axId val="100722944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12510,7 +12508,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102629760"/>
+        <c:crossAx val="100729216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12518,7 +12516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102629760"/>
+        <c:axId val="100729216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12529,7 +12527,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102623488"/>
+        <c:crossAx val="100722944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12586,7 +12584,7 @@
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
@@ -12900,8 +12898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+    <sheetView tabSelected="1" topLeftCell="U7" workbookViewId="0">
+      <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12909,10 +12907,13 @@
     <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.140625" customWidth="1"/>
     <col min="26" max="26" width="13.42578125" customWidth="1"/>
+    <col min="27" max="28" width="12" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="15.7109375" customWidth="1"/>
-    <col min="30" max="31" width="15" customWidth="1"/>
-    <col min="32" max="32" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15" customWidth="1"/>
+    <col min="31" max="31" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -12929,37 +12930,37 @@
         <v>3</v>
       </c>
       <c r="X1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD1" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AE1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>4</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -12983,28 +12984,28 @@
         <v>4.0023969999999999E-2</v>
       </c>
       <c r="Z2">
-        <v>2.47041E-2</v>
+        <v>2.5553800000000002E-2</v>
       </c>
       <c r="AA2">
-        <v>2.4629600000000001E-2</v>
+        <v>3.1666699999999999E-2</v>
       </c>
       <c r="AB2">
-        <v>2.7544900000000001E-2</v>
+        <v>3.5593800000000002E-2</v>
       </c>
       <c r="AC2">
-        <v>2.4692499999999999E-2</v>
+        <v>2.40538E-2</v>
       </c>
       <c r="AD2">
-        <v>2.89968E-2</v>
+        <v>2.8556999999999999E-2</v>
       </c>
       <c r="AE2">
-        <v>2.6776299999999999E-2</v>
+        <v>2.4276499999999999E-2</v>
       </c>
       <c r="AF2">
-        <v>2.6374100000000001E-2</v>
+        <v>3.4881599999999999E-2</v>
       </c>
       <c r="AG2">
-        <v>2.28281E-2</v>
+        <v>6.1439599999999999</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -13028,28 +13029,28 @@
         <v>1.764429E-2</v>
       </c>
       <c r="Z3">
-        <v>2.9869900000000001E-2</v>
+        <v>2.7735800000000001E-2</v>
       </c>
       <c r="AA3">
-        <v>3.1960200000000001E-2</v>
+        <v>3.0497099999999999E-2</v>
       </c>
       <c r="AB3">
-        <v>2.4779099999999998E-2</v>
+        <v>3.0673599999999999E-2</v>
       </c>
       <c r="AC3">
-        <v>2.7592999999999999E-2</v>
+        <v>2.43162E-2</v>
       </c>
       <c r="AD3">
-        <v>2.7449299999999999E-2</v>
+        <v>2.5625700000000001E-2</v>
       </c>
       <c r="AE3">
-        <v>2.5118499999999998E-2</v>
+        <v>2.3868400000000001E-2</v>
       </c>
       <c r="AF3">
-        <v>2.7071399999999999E-2</v>
+        <v>3.1811100000000002E-2</v>
       </c>
       <c r="AG3">
-        <v>2.30572E-2</v>
+        <v>6.1433200000000001</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
@@ -13073,25 +13074,28 @@
         <v>4.3591709999999999E-2</v>
       </c>
       <c r="Z4">
-        <v>2.43891E-2</v>
+        <v>2.6452E-2</v>
       </c>
       <c r="AA4">
-        <v>2.8483499999999998E-2</v>
+        <v>2.8981699999999999E-2</v>
       </c>
       <c r="AB4">
-        <v>2.76841E-2</v>
+        <v>2.69865E-2</v>
       </c>
       <c r="AC4">
-        <v>2.6224600000000001E-2</v>
+        <v>2.7874400000000001E-2</v>
+      </c>
+      <c r="AD4">
+        <v>2.7539500000000001E-2</v>
       </c>
       <c r="AE4">
-        <v>2.71138E-2</v>
+        <v>2.2632099999999999E-2</v>
       </c>
       <c r="AF4">
-        <v>2.79902E-2</v>
+        <v>3.2640000000000002E-2</v>
       </c>
       <c r="AG4">
-        <v>2.57177E-2</v>
+        <v>6.1372900000000001</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
@@ -13115,25 +13119,28 @@
         <v>3.9400369999999997E-2</v>
       </c>
       <c r="Z5">
-        <v>2.8991599999999999E-2</v>
+        <v>2.7638300000000001E-2</v>
       </c>
       <c r="AA5">
-        <v>2.6041100000000001E-2</v>
+        <v>2.5240100000000001E-2</v>
       </c>
       <c r="AB5">
-        <v>2.48548E-2</v>
+        <v>2.5638500000000002E-2</v>
       </c>
       <c r="AC5">
-        <v>2.5333399999999999E-2</v>
+        <v>2.2243300000000001E-2</v>
+      </c>
+      <c r="AD5">
+        <v>2.5050200000000002E-2</v>
       </c>
       <c r="AE5">
-        <v>2.89108E-2</v>
+        <v>2.4959100000000001E-2</v>
       </c>
       <c r="AF5">
-        <v>2.79902E-2</v>
+        <v>3.4500500000000003E-2</v>
       </c>
       <c r="AG5">
-        <v>3.3609E-2</v>
+        <v>6.1533699999999998</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -13157,25 +13164,28 @@
         <v>4.0634099999999999E-2</v>
       </c>
       <c r="Z6">
-        <v>2.8546999999999999E-2</v>
+        <v>2.7638300000000001E-2</v>
       </c>
       <c r="AA6">
-        <v>2.6856499999999998E-2</v>
+        <v>2.5240700000000001E-2</v>
       </c>
       <c r="AB6">
-        <v>2.9156499999999998E-2</v>
+        <v>2.8676400000000001E-2</v>
       </c>
       <c r="AC6">
-        <v>2.4306899999999999E-2</v>
+        <v>2.18911E-2</v>
+      </c>
+      <c r="AD6">
+        <v>2.3124200000000001E-2</v>
       </c>
       <c r="AE6">
-        <v>2.42518E-2</v>
+        <v>2.0014500000000001E-2</v>
       </c>
       <c r="AF6">
-        <v>2.6009600000000001E-2</v>
+        <v>3.4500500000000003E-2</v>
       </c>
       <c r="AG6">
-        <v>2.8070299999999999E-2</v>
+        <v>6.13436</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -13198,27 +13208,6 @@
       <c r="Y7">
         <v>3.6535140000000001E-2</v>
       </c>
-      <c r="Z7">
-        <v>2.7404399999999999E-2</v>
-      </c>
-      <c r="AA7">
-        <v>2.76963E-2</v>
-      </c>
-      <c r="AB7">
-        <v>2.92765E-2</v>
-      </c>
-      <c r="AC7">
-        <v>2.59898E-2</v>
-      </c>
-      <c r="AE7">
-        <v>3.3163100000000001E-2</v>
-      </c>
-      <c r="AF7">
-        <v>3.0710399999999999E-2</v>
-      </c>
-      <c r="AG7">
-        <v>2.3626899999999999E-2</v>
-      </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -13240,18 +13229,6 @@
       <c r="Y8">
         <v>3.9424109999999998E-2</v>
       </c>
-      <c r="Z8">
-        <v>2.7390899999999999E-2</v>
-      </c>
-      <c r="AA8">
-        <v>3.0354300000000001E-2</v>
-      </c>
-      <c r="AB8">
-        <v>2.68142E-2</v>
-      </c>
-      <c r="AC8">
-        <v>2.8063899999999999E-2</v>
-      </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -13273,18 +13250,6 @@
       <c r="Y9">
         <v>3.8635620000000002E-2</v>
       </c>
-      <c r="Z9">
-        <v>2.8489299999999999E-2</v>
-      </c>
-      <c r="AA9">
-        <v>2.7296000000000001E-2</v>
-      </c>
-      <c r="AB9">
-        <v>2.52263E-2</v>
-      </c>
-      <c r="AC9">
-        <v>2.9552999999999999E-2</v>
-      </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -13306,18 +13271,6 @@
       <c r="Y10">
         <v>1.9983440000000002E-2</v>
       </c>
-      <c r="Z10">
-        <v>2.6776999999999999E-2</v>
-      </c>
-      <c r="AA10">
-        <v>2.8030599999999999E-2</v>
-      </c>
-      <c r="AB10">
-        <v>2.8394300000000001E-2</v>
-      </c>
-      <c r="AC10">
-        <v>2.66243E-2</v>
-      </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -13339,18 +13292,6 @@
       <c r="Y11">
         <v>3.9596689999999997E-2</v>
       </c>
-      <c r="Z11">
-        <v>2.9503000000000001E-2</v>
-      </c>
-      <c r="AA11">
-        <v>2.69252E-2</v>
-      </c>
-      <c r="AB11">
-        <v>3.5244999999999999E-2</v>
-      </c>
-      <c r="AC11">
-        <v>2.6069999999999999E-2</v>
-      </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -13382,7 +13323,7 @@
         <v>-4.9999999998107114E-6</v>
       </c>
       <c r="W13" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="X13">
         <f>AVERAGE(X2:X11)</f>
@@ -13394,35 +13335,35 @@
       </c>
       <c r="Z13">
         <f>AVERAGE(Z2:Z11)</f>
-        <v>2.760663E-2</v>
+        <v>2.7003640000000002E-2</v>
       </c>
       <c r="AA13">
         <f t="shared" ref="AA13:AC13" si="1">AVERAGE(AA2:AA11)</f>
-        <v>2.7827330000000001E-2</v>
+        <v>2.8325259999999998E-2</v>
       </c>
       <c r="AB13">
         <f t="shared" si="1"/>
-        <v>2.7897570000000003E-2</v>
+        <v>2.951376E-2</v>
       </c>
       <c r="AC13">
         <f t="shared" si="1"/>
-        <v>2.6445139999999999E-2</v>
+        <v>2.4075759999999995E-2</v>
       </c>
       <c r="AD13">
-        <f t="shared" ref="AD13:AG13" si="2">AVERAGE(AD2:AD11)</f>
-        <v>2.822305E-2</v>
+        <f t="shared" ref="AD13" si="2">AVERAGE(AD2:AD11)</f>
+        <v>2.597932E-2</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="2"/>
-        <v>2.7555716666666664E-2</v>
+        <f>AVERAGE(AE2:AE6)</f>
+        <v>2.3150120000000003E-2</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="2"/>
-        <v>2.7690983333333332E-2</v>
+        <f>AVERAGE(AF2:AF6)</f>
+        <v>3.3666739999999994E-2</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="2"/>
-        <v>2.6151533333333334E-2</v>
+        <f>AVERAGE(AG2:AG6)</f>
+        <v>6.1424599999999998</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
@@ -13440,7 +13381,7 @@
         <v>-1.0000000010279564E-6</v>
       </c>
       <c r="W14" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="X14">
         <f>_xlfn.STDEV.P(X2:X11)</f>
@@ -13452,35 +13393,35 @@
       </c>
       <c r="Z14">
         <f>_xlfn.STDEV.P(Z2:Z11)</f>
-        <v>1.7847424542773674E-3</v>
+        <v>8.6579300205072126E-4</v>
       </c>
       <c r="AA14">
         <f t="shared" ref="AA14:AC14" si="3">_xlfn.STDEV.P(AA2:AA11)</f>
-        <v>1.9851950584514359E-3</v>
+        <v>2.6587871803512206E-3</v>
       </c>
       <c r="AB14">
         <f t="shared" si="3"/>
-        <v>2.9185689120012222E-3</v>
+        <v>3.4761464345450122E-3</v>
       </c>
       <c r="AC14">
         <f t="shared" si="3"/>
-        <v>1.513451159568752E-3</v>
+        <v>2.1269042504071501E-3</v>
       </c>
       <c r="AD14">
-        <f t="shared" ref="AD14:AG14" si="4">_xlfn.STDEV.P(AD2:AD11)</f>
-        <v>7.7375000000000013E-4</v>
+        <f t="shared" ref="AD14" si="4">_xlfn.STDEV.P(AD2:AD11)</f>
+        <v>1.9088539550211792E-3</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="4"/>
-        <v>2.9136938122233933E-3</v>
+        <f>_xlfn.STDEV.P(AE2:AE6)</f>
+        <v>1.7411217193522112E-3</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="4"/>
-        <v>1.5406196463508507E-3</v>
+        <f>_xlfn.STDEV.P(AF2:AF6)</f>
+        <v>1.2135725056213161E-3</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="4"/>
-        <v>3.7964362089845378E-3</v>
+        <f>_xlfn.STDEV.P(AG2:AG6)</f>
+        <v>6.5476194147184993E-3</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -13498,7 +13439,7 @@
         <v>2.0000000002795559E-6</v>
       </c>
       <c r="W15" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="X15">
         <v>100</v>
@@ -13519,15 +13460,12 @@
         <v>1024</v>
       </c>
       <c r="AD15">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="AE15">
-        <v>4096</v>
+        <v>8192</v>
       </c>
       <c r="AF15">
-        <v>8192</v>
-      </c>
-      <c r="AG15">
         <v>16384</v>
       </c>
     </row>
@@ -13546,18 +13484,18 @@
         <v>-4.9999999998107114E-6</v>
       </c>
       <c r="W16" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="X16">
         <f>((X13-Z13)/X13)*100</f>
-        <v>59.018539731447376</v>
+        <v>59.913665675010009</v>
       </c>
       <c r="Y16">
         <f>((Y13-Z13)/Y13)*100</f>
-        <v>22.337543277981919</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24.033863501740107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -13572,7 +13510,7 @@
         <v>-4.0000000005591119E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3.2000000000000002E-3</v>
       </c>
@@ -13587,7 +13525,7 @@
         <v>-3.0000000000640625E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3.3999999999999998E-3</v>
       </c>
@@ -13602,7 +13540,7 @@
         <v>-1.9999999999242846E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3.5999999999999999E-3</v>
       </c>
@@ -13617,7 +13555,7 @@
         <v>-1.9999999999242846E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3.8E-3</v>
       </c>
@@ -13631,8 +13569,14 @@
         <f t="shared" si="0"/>
         <v>4.0000000000262048E-5</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="W21" t="s">
+        <v>11</v>
+      </c>
+      <c r="X21" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4.0000000000000001E-3</v>
       </c>
@@ -13646,8 +13590,14 @@
         <f t="shared" si="0"/>
         <v>-2.0000000001019203E-5</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="W22" t="s">
+        <v>12</v>
+      </c>
+      <c r="X22">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4.1999999999999997E-3</v>
       </c>
@@ -13662,7 +13612,7 @@
         <v>9.9999999996214228E-6</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4.4000000000000003E-3</v>
       </c>
@@ -13677,7 +13627,7 @@
         <v>-9.9999999996214228E-6</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4.5999999999999999E-3</v>
       </c>
@@ -13692,7 +13642,7 @@
         <v>-3.0000000000640625E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4.7999999999999996E-3</v>
       </c>
@@ -13707,7 +13657,7 @@
         <v>-4.0000000000262048E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -13722,7 +13672,7 @@
         <v>-4.9999999999883471E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5.1999999999999998E-3</v>
       </c>
@@ -13737,7 +13687,7 @@
         <v>-9.9999999996214228E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5.4000000000000003E-3</v>
       </c>
@@ -13752,7 +13702,7 @@
         <v>9.9999999996214228E-6</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5.5999999999999999E-3</v>
       </c>
@@ -13767,7 +13717,7 @@
         <v>-9.9999999996214228E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5.7999999999999996E-3</v>
       </c>
@@ -13782,7 +13732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6.0000000000000001E-3</v>
       </c>

</xml_diff>

<commit_message>
Got the 2D Vm array working. It is not really 2D, It is just interleaved with an active array index that tells which part of the 1D array to use. It got me another 30-41% increase in performance.
</commit_message>
<xml_diff>
--- a/Libraries/OpenNeuronCL/PerformanceStats.xlsx
+++ b/Libraries/OpenNeuronCL/PerformanceStats.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="4560" yWindow="1305" windowWidth="11010" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="FastSpiking Phase 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Comparisons" sheetId="2" r:id="rId1"/>
+    <sheet name="FastSpiking Phase 1" sheetId="1" r:id="rId2"/>
+    <sheet name="FastSpiking Single Vm" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>Time</t>
   </si>
@@ -79,6 +80,36 @@
   </si>
   <si>
     <t>OCL 2^24</t>
+  </si>
+  <si>
+    <t>Stdev</t>
+  </si>
+  <si>
+    <t>FS1 OCL 2^10</t>
+  </si>
+  <si>
+    <t>FS1 OCL 2^16</t>
+  </si>
+  <si>
+    <t>FS1 OCL 2^20</t>
+  </si>
+  <si>
+    <t>FS1 OCL 2^23</t>
+  </si>
+  <si>
+    <t>FS2 OCL 2^10</t>
+  </si>
+  <si>
+    <t>FS2 OCL 2^16</t>
+  </si>
+  <si>
+    <t>FS2 OCL 2^20</t>
+  </si>
+  <si>
+    <t>FS2 OCL 2^23</t>
+  </si>
+  <si>
+    <t>FS1-FS2 %</t>
   </si>
 </sst>
 </file>
@@ -12233,11 +12264,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="100680448"/>
-        <c:axId val="100681984"/>
+        <c:axId val="96023296"/>
+        <c:axId val="96024832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100680448"/>
+        <c:axId val="96023296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12247,12 +12278,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100681984"/>
+        <c:crossAx val="96024832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100681984"/>
+        <c:axId val="96024832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12263,7 +12294,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100680448"/>
+        <c:crossAx val="96023296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12471,11 +12502,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="100722944"/>
-        <c:axId val="100729216"/>
+        <c:axId val="96073984"/>
+        <c:axId val="96076160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="100722944"/>
+        <c:axId val="96073984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12508,7 +12539,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100729216"/>
+        <c:crossAx val="96076160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12516,7 +12547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100729216"/>
+        <c:axId val="96076160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12527,7 +12558,266 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100722944"/>
+        <c:crossAx val="96073984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'FastSpiking Single Vm'!$B$14:$J$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>9.9474631418057582E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.5449813137914027E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.153950561505994E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.0439739774534616E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8.2713260025222071E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.3517693807301246E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'FastSpiking Single Vm'!$B$14:$J$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>9.9474631418057582E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.5449813137914027E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.153950561505994E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.0439739774534616E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8.2713260025222071E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3.3517693807301246E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FastSpiking Single Vm'!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>V2_IGF_100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FSP_100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCL 2^10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OCL 2^12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>OCL 2^14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>OCL 2^16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>OCL 2^18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>OCL 2^20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>OCL 2^23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCL 2^24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'FastSpiking Single Vm'!$B$13:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.736370500000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5546943999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5872959999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7087979999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7595339999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.4541420000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="39283328"/>
+        <c:axId val="39293696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="39283328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>AnimatLab</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> 100 Neurons Comparison with OPenCL</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39293696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="39293696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="39283328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12601,6 +12891,43 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -12896,10 +13223,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <f>'FastSpiking Phase 1'!X13</f>
+        <v>6.736370500000001E-2</v>
+      </c>
+      <c r="C2">
+        <f>'FastSpiking Phase 1'!X14</f>
+        <v>9.9474631418057582E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f>'FastSpiking Phase 1'!Y13</f>
+        <v>3.5546943999999997E-2</v>
+      </c>
+      <c r="C3">
+        <f>'FastSpiking Phase 1'!Y14</f>
+        <v>8.5449813137914027E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <f>'FastSpiking Phase 1'!Z13</f>
+        <v>2.7003640000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <f>'FastSpiking Phase 1'!AC13</f>
+        <v>2.4075759999999995E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <f>'FastSpiking Phase 1'!AE13</f>
+        <v>2.3150120000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8">
+        <f>'FastSpiking Phase 1'!AF13</f>
+        <v>3.3666739999999994E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <f>'FastSpiking Single Vm'!D13</f>
+        <v>1.5872959999999998E-2</v>
+      </c>
+      <c r="O10">
+        <f>((B5-B10)/B5)*100</f>
+        <v>41.219183784112076</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <f>'FastSpiking Single Vm'!G13</f>
+        <v>1.7087979999999999E-2</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ref="O11:O13" si="0">((B6-B11)/B6)*100</f>
+        <v>29.024130494738266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <f>'FastSpiking Single Vm'!I13</f>
+        <v>1.7595339999999998E-2</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>23.994605643512884</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <f>'FastSpiking Single Vm'!J13</f>
+        <v>3.4541420000000003E-2</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="0"/>
+        <v>-2.5980537468136502</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U7" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28288,19 +28758,361 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>7.2041859999999999E-2</v>
+      </c>
+      <c r="C2">
+        <v>4.0023969999999999E-2</v>
+      </c>
+      <c r="D2">
+        <v>1.6894599999999999E-2</v>
+      </c>
+      <c r="G2">
+        <v>1.66572E-2</v>
+      </c>
+      <c r="I2">
+        <v>1.7504100000000002E-2</v>
+      </c>
+      <c r="J2">
+        <v>3.4194700000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>5.2445930000000002E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.764429E-2</v>
+      </c>
+      <c r="D3">
+        <v>1.7364299999999999E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.8242600000000001E-2</v>
+      </c>
+      <c r="I3">
+        <v>1.6397999999999999E-2</v>
+      </c>
+      <c r="J3">
+        <v>3.58686E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>7.4952640000000001E-2</v>
+      </c>
+      <c r="C4">
+        <v>4.3591709999999999E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.47408E-2</v>
+      </c>
+      <c r="G4">
+        <v>1.5493399999999999E-2</v>
+      </c>
+      <c r="I4">
+        <v>1.7299499999999999E-2</v>
+      </c>
+      <c r="J4">
+        <v>3.5006299999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>7.2751430000000006E-2</v>
+      </c>
+      <c r="C5">
+        <v>3.9400369999999997E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.4422600000000001E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.6813100000000001E-2</v>
+      </c>
+      <c r="I5">
+        <v>1.7823599999999998E-2</v>
+      </c>
+      <c r="J5">
+        <v>3.8968000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>7.2371619999999998E-2</v>
+      </c>
+      <c r="C6">
+        <v>4.0634099999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>1.5942499999999998E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.8233599999999999E-2</v>
+      </c>
+      <c r="I6">
+        <v>1.89515E-2</v>
+      </c>
+      <c r="J6">
+        <v>2.8669500000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>7.2689199999999995E-2</v>
+      </c>
+      <c r="C7">
+        <v>3.6535140000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4.8488759999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>3.9424109999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7.4415010000000004E-2</v>
+      </c>
+      <c r="C9">
+        <v>3.8635620000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>5.6783550000000002E-2</v>
+      </c>
+      <c r="C10">
+        <v>1.9983440000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>7.6697050000000003E-2</v>
+      </c>
+      <c r="C11">
+        <v>3.9596689999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(B2:B11)</f>
+        <v>6.736370500000001E-2</v>
+      </c>
+      <c r="C13">
+        <f>AVERAGE(C2:C11)</f>
+        <v>3.5546943999999997E-2</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(D2:D11)</f>
+        <v>1.5872959999999998E-2</v>
+      </c>
+      <c r="E13" t="e">
+        <f t="shared" ref="E13:H13" si="0">AVERAGE(E2:E11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1.7087979999999999E-2</v>
+      </c>
+      <c r="H13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13">
+        <f>AVERAGE(I2:I6)</f>
+        <v>1.7595339999999998E-2</v>
+      </c>
+      <c r="J13">
+        <f>AVERAGE(J2:J6)</f>
+        <v>3.4541420000000003E-2</v>
+      </c>
+      <c r="K13" t="e">
+        <f>AVERAGE(K2:K6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <f>_xlfn.STDEV.P(B2:B11)</f>
+        <v>9.9474631418057582E-3</v>
+      </c>
+      <c r="C14">
+        <f>_xlfn.STDEV.P(C2:C11)</f>
+        <v>8.5449813137914027E-3</v>
+      </c>
+      <c r="D14">
+        <f>_xlfn.STDEV.P(D2:D11)</f>
+        <v>1.153950561505994E-3</v>
+      </c>
+      <c r="E14" t="e">
+        <f t="shared" ref="E14:H14" si="1">_xlfn.STDEV.P(E2:E11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>1.0439739774534616E-3</v>
+      </c>
+      <c r="H14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14">
+        <f>_xlfn.STDEV.P(I2:I6)</f>
+        <v>8.2713260025222071E-4</v>
+      </c>
+      <c r="J14">
+        <f>_xlfn.STDEV.P(J2:J6)</f>
+        <v>3.3517693807301246E-3</v>
+      </c>
+      <c r="K14" t="e">
+        <f>_xlfn.STDEV.P(K2:K6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>256</v>
+      </c>
+      <c r="F15">
+        <v>512</v>
+      </c>
+      <c r="G15">
+        <v>1024</v>
+      </c>
+      <c r="H15">
+        <v>4096</v>
+      </c>
+      <c r="I15">
+        <v>8192</v>
+      </c>
+      <c r="J15">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <f>((B13-D13)/B13)*100</f>
+        <v>76.436925492741238</v>
+      </c>
+      <c r="C16">
+        <f>((C13-D13)/C13)*100</f>
+        <v>55.346484918647299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
i now have a random number generating framework for use in the Kernels. It can generate random ints or floats within a specified range using the global id, timeslice, and a seed value. I tested this using the threefry and philox generation methods and did not find any significant increase in processing time.
</commit_message>
<xml_diff>
--- a/Libraries/OpenNeuronCL/PerformanceStats.xlsx
+++ b/Libraries/OpenNeuronCL/PerformanceStats.xlsx
@@ -10,14 +10,15 @@
     <sheet name="Comparisons" sheetId="2" r:id="rId1"/>
     <sheet name="FastSpiking Phase 1" sheetId="1" r:id="rId2"/>
     <sheet name="FastSpiking Single Vm" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="FastSpiking ThreeFry Random Num" sheetId="5" r:id="rId4"/>
+    <sheet name="FastSpiking Philox Random " sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="35">
   <si>
     <t>Time</t>
   </si>
@@ -111,6 +112,18 @@
   <si>
     <t>FS1-FS2 %</t>
   </si>
+  <si>
+    <t>Fast spiking phase 1</t>
+  </si>
+  <si>
+    <t>Fast Spiking Single Vm</t>
+  </si>
+  <si>
+    <t>Fast Spiking Threefry Random</t>
+  </si>
+  <si>
+    <t>Fast Spiking Philox Random</t>
+  </si>
 </sst>
 </file>
 
@@ -12264,11 +12277,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="96023296"/>
-        <c:axId val="96024832"/>
+        <c:axId val="103904384"/>
+        <c:axId val="103905920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96023296"/>
+        <c:axId val="103904384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12278,12 +12291,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96024832"/>
+        <c:crossAx val="103905920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96024832"/>
+        <c:axId val="103905920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12294,14 +12307,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96023296"/>
+        <c:crossAx val="103904384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12502,11 +12514,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="96073984"/>
-        <c:axId val="96076160"/>
+        <c:axId val="104307328"/>
+        <c:axId val="104313600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96073984"/>
+        <c:axId val="104307328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12533,13 +12545,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96076160"/>
+        <c:crossAx val="104313600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12547,7 +12558,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96076160"/>
+        <c:axId val="104313600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12558,7 +12569,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96073984"/>
+        <c:crossAx val="104307328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12761,11 +12772,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="39283328"/>
-        <c:axId val="39293696"/>
+        <c:axId val="104149760"/>
+        <c:axId val="104151680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39283328"/>
+        <c:axId val="104149760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12798,7 +12809,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39293696"/>
+        <c:crossAx val="104151680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12806,7 +12817,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39293696"/>
+        <c:axId val="104151680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12817,7 +12828,525 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39283328"/>
+        <c:crossAx val="104149760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'FastSpiking ThreeFry Random Num'!$B$14:$J$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>9.9474631418057582E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.5449813137914027E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.4757330414407615E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.9347408839813764E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.6261718603320678E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4.3044961490980556E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'FastSpiking ThreeFry Random Num'!$B$14:$J$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>9.9474631418057582E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.5449813137914027E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.4757330414407615E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.9347408839813764E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2.6261718603320678E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4.3044961490980556E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FastSpiking ThreeFry Random Num'!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>V2_IGF_100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FSP_100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCL 2^10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OCL 2^12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>OCL 2^14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>OCL 2^16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>OCL 2^18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>OCL 2^20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>OCL 2^23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCL 2^24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'FastSpiking ThreeFry Random Num'!$B$13:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.736370500000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5546943999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4799619999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.425392E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1926639999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.6706219999999996E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="41153664"/>
+        <c:axId val="41155584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="41153664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>AnimatLab</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> 100 Neurons Comparison with OPenCL</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="41155584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="41155584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="41153664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'FastSpiking Philox Random '!$B$14:$J$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>9.9474631418057582E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.5449813137914027E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.8065069527682426E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.408038093854539E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.1233860110236399E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.3468811069732137E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'FastSpiking Philox Random '!$B$14:$J$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>9.9474631418057582E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.5449813137914027E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.8065069527682426E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.408038093854539E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.1233860110236399E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.3468811069732137E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FastSpiking Philox Random '!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>V2_IGF_100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FSP_100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCL 2^10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OCL 2^12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>OCL 2^14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>OCL 2^16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>OCL 2^18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>OCL 2^20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>OCL 2^23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCL 2^24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'FastSpiking Philox Random '!$B$13:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.736370500000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5546943999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.512374E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.35409E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2524159999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3581599999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="37876096"/>
+        <c:axId val="37878016"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="37876096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>AnimatLab</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> 100 Neurons Comparison with OPenCL</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="37878016"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="37878016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="37876096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12917,6 +13446,80 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -13223,10 +13826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13234,18 +13837,18 @@
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -13258,7 +13861,7 @@
         <v>9.9474631418057582E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -13271,92 +13874,216 @@
         <v>8.5449813137914027E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <f>'FastSpiking Phase 1'!Z13</f>
         <v>2.7003640000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <f>'FastSpiking Phase 1'!AC13</f>
         <v>2.4075759999999995E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <f>'FastSpiking Phase 1'!AE13</f>
         <v>2.3150120000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <f>'FastSpiking Phase 1'!AF13</f>
         <v>3.3666739999999994E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B10">
+      <c r="B12">
         <f>'FastSpiking Single Vm'!D13</f>
         <v>1.5872959999999998E-2</v>
       </c>
-      <c r="O10">
-        <f>((B5-B10)/B5)*100</f>
+      <c r="F12">
+        <f>(($B$6-B12)/$B$6)*100</f>
         <v>41.219183784112076</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <f>'FastSpiking Single Vm'!G13</f>
         <v>1.7087979999999999E-2</v>
       </c>
-      <c r="O11">
-        <f t="shared" ref="O11:O13" si="0">((B6-B11)/B6)*100</f>
+      <c r="F13">
+        <f>(($B$7-B13)/$B$7)*100</f>
         <v>29.024130494738266</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B12">
+      <c r="B14">
         <f>'FastSpiking Single Vm'!I13</f>
         <v>1.7595339999999998E-2</v>
       </c>
-      <c r="O12">
-        <f t="shared" si="0"/>
+      <c r="F14">
+        <f>(($B$8-B14)/$B$8)*100</f>
         <v>23.994605643512884</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B13">
+      <c r="B15">
         <f>'FastSpiking Single Vm'!J13</f>
         <v>3.4541420000000003E-2</v>
       </c>
-      <c r="O13">
-        <f t="shared" si="0"/>
+      <c r="F15">
+        <f>(($B$9-B15)/$B$9)*100</f>
         <v>-2.5980537468136502</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <f>'FastSpiking ThreeFry Random Num'!D13</f>
+        <v>1.4799619999999999E-2</v>
+      </c>
+      <c r="F18">
+        <f>(($B$6-B18)/$B$6)*100</f>
+        <v>45.193981255860329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <f>'FastSpiking ThreeFry Random Num'!G13</f>
+        <v>1.425392E-2</v>
+      </c>
+      <c r="F19">
+        <f>(($B$7-B19)/$B$7)*100</f>
+        <v>40.795555363568987</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <f>'FastSpiking ThreeFry Random Num'!I13</f>
+        <v>1.1926639999999999E-2</v>
+      </c>
+      <c r="F20">
+        <f>(($B$8-B20)/$B$8)*100</f>
+        <v>48.481303768619789</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <f>'FastSpiking ThreeFry Random Num'!J13</f>
+        <v>2.6706219999999996E-2</v>
+      </c>
+      <c r="F21">
+        <f>(($B$9-B21)/$B$9)*100</f>
+        <v>20.674766847042509</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <f>'FastSpiking Philox Random '!D13</f>
+        <v>1.512374E-2</v>
+      </c>
+      <c r="F24">
+        <f>(($B$6-B24)/$B$6)*100</f>
+        <v>43.993698627296176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <f>'FastSpiking Philox Random '!G13</f>
+        <v>1.35409E-2</v>
+      </c>
+      <c r="F25">
+        <f>(($B$7-B25)/$B$7)*100</f>
+        <v>43.757123347300343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <f>'FastSpiking Philox Random '!I13</f>
+        <v>1.2524159999999998E-2</v>
+      </c>
+      <c r="F26">
+        <f>(($B$8-B26)/$B$8)*100</f>
+        <v>45.900237234191458</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <f>'FastSpiking Philox Random '!J13</f>
+        <v>2.3581599999999998E-2</v>
+      </c>
+      <c r="F27">
+        <f>(($B$9-B27)/$B$9)*100</f>
+        <v>29.955796135889599</v>
       </c>
     </row>
   </sheetData>
@@ -29114,12 +29841,702 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>7.2041859999999999E-2</v>
+      </c>
+      <c r="C2">
+        <v>4.0023969999999999E-2</v>
+      </c>
+      <c r="D2">
+        <v>1.44926E-2</v>
+      </c>
+      <c r="G2">
+        <v>1.5013500000000001E-2</v>
+      </c>
+      <c r="I2">
+        <v>1.21952E-2</v>
+      </c>
+      <c r="J2">
+        <v>2.27493E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>5.2445930000000002E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.764429E-2</v>
+      </c>
+      <c r="D3">
+        <v>1.3081199999999999E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.4817200000000001E-2</v>
+      </c>
+      <c r="I3">
+        <v>1.16223E-2</v>
+      </c>
+      <c r="J3">
+        <v>3.0997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>7.4952640000000001E-2</v>
+      </c>
+      <c r="C4">
+        <v>4.3591709999999999E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.75354E-2</v>
+      </c>
+      <c r="G4">
+        <v>1.34436E-2</v>
+      </c>
+      <c r="I4">
+        <v>1.15934E-2</v>
+      </c>
+      <c r="J4">
+        <v>3.2831199999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>7.2751430000000006E-2</v>
+      </c>
+      <c r="C5">
+        <v>3.9400369999999997E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.4673500000000001E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.37991E-2</v>
+      </c>
+      <c r="I5">
+        <v>1.2133E-2</v>
+      </c>
+      <c r="J5">
+        <v>2.37944E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>7.2371619999999998E-2</v>
+      </c>
+      <c r="C6">
+        <v>4.0634099999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>1.42154E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.4196200000000001E-2</v>
+      </c>
+      <c r="I6">
+        <v>1.2089300000000001E-2</v>
+      </c>
+      <c r="J6">
+        <v>2.3159200000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>7.2689199999999995E-2</v>
+      </c>
+      <c r="C7">
+        <v>3.6535140000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4.8488759999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>3.9424109999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7.4415010000000004E-2</v>
+      </c>
+      <c r="C9">
+        <v>3.8635620000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>5.6783550000000002E-2</v>
+      </c>
+      <c r="C10">
+        <v>1.9983440000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>7.6697050000000003E-2</v>
+      </c>
+      <c r="C11">
+        <v>3.9596689999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(B2:B11)</f>
+        <v>6.736370500000001E-2</v>
+      </c>
+      <c r="C13">
+        <f>AVERAGE(C2:C11)</f>
+        <v>3.5546943999999997E-2</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(D2:D11)</f>
+        <v>1.4799619999999999E-2</v>
+      </c>
+      <c r="E13" t="e">
+        <f t="shared" ref="E13:H13" si="0">AVERAGE(E2:E11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1.425392E-2</v>
+      </c>
+      <c r="H13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13">
+        <f>AVERAGE(I2:I6)</f>
+        <v>1.1926639999999999E-2</v>
+      </c>
+      <c r="J13">
+        <f>AVERAGE(J2:J6)</f>
+        <v>2.6706219999999996E-2</v>
+      </c>
+      <c r="K13" t="e">
+        <f>AVERAGE(K2:K6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <f>_xlfn.STDEV.P(B2:B11)</f>
+        <v>9.9474631418057582E-3</v>
+      </c>
+      <c r="C14">
+        <f>_xlfn.STDEV.P(C2:C11)</f>
+        <v>8.5449813137914027E-3</v>
+      </c>
+      <c r="D14">
+        <f>_xlfn.STDEV.P(D2:D11)</f>
+        <v>1.4757330414407615E-3</v>
+      </c>
+      <c r="E14" t="e">
+        <f t="shared" ref="E14:H14" si="1">_xlfn.STDEV.P(E2:E11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>5.9347408839813764E-4</v>
+      </c>
+      <c r="H14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14">
+        <f>_xlfn.STDEV.P(I2:I6)</f>
+        <v>2.6261718603320678E-4</v>
+      </c>
+      <c r="J14">
+        <f>_xlfn.STDEV.P(J2:J6)</f>
+        <v>4.3044961490980556E-3</v>
+      </c>
+      <c r="K14" t="e">
+        <f>_xlfn.STDEV.P(K2:K6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>256</v>
+      </c>
+      <c r="F15">
+        <v>512</v>
+      </c>
+      <c r="G15">
+        <v>1024</v>
+      </c>
+      <c r="H15">
+        <v>4096</v>
+      </c>
+      <c r="I15">
+        <v>8192</v>
+      </c>
+      <c r="J15">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <f>((B13-D13)/B13)*100</f>
+        <v>78.030276096007483</v>
+      </c>
+      <c r="C16">
+        <f>((C13-D13)/C13)*100</f>
+        <v>58.365984991564957</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>7.2041859999999999E-2</v>
+      </c>
+      <c r="C2">
+        <v>4.0023969999999999E-2</v>
+      </c>
+      <c r="D2">
+        <v>1.44926E-2</v>
+      </c>
+      <c r="G2">
+        <v>1.40307E-2</v>
+      </c>
+      <c r="I2">
+        <v>1.34699E-2</v>
+      </c>
+      <c r="J2">
+        <v>2.4549499999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>5.2445930000000002E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.764429E-2</v>
+      </c>
+      <c r="D3">
+        <v>1.4234699999999999E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.24133E-2</v>
+      </c>
+      <c r="I3">
+        <v>1.2516599999999999E-2</v>
+      </c>
+      <c r="J3">
+        <v>2.3424799999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>7.4952640000000001E-2</v>
+      </c>
+      <c r="C4">
+        <v>4.3591709999999999E-2</v>
+      </c>
+      <c r="D4">
+        <v>1.8427200000000001E-2</v>
+      </c>
+      <c r="G4">
+        <v>1.3573200000000001E-2</v>
+      </c>
+      <c r="I4">
+        <v>1.1624199999999999E-2</v>
+      </c>
+      <c r="J4">
+        <v>2.2770499999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>7.2751430000000006E-2</v>
+      </c>
+      <c r="C5">
+        <v>3.9400369999999997E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.53779E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.31197E-2</v>
+      </c>
+      <c r="I5">
+        <v>1.27963E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>7.2371619999999998E-2</v>
+      </c>
+      <c r="C6">
+        <v>4.0634099999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>1.30863E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.45676E-2</v>
+      </c>
+      <c r="I6">
+        <v>1.22138E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>7.2689199999999995E-2</v>
+      </c>
+      <c r="C7">
+        <v>3.6535140000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>4.8488759999999999E-2</v>
+      </c>
+      <c r="C8">
+        <v>3.9424109999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7.4415010000000004E-2</v>
+      </c>
+      <c r="C9">
+        <v>3.8635620000000002E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>5.6783550000000002E-2</v>
+      </c>
+      <c r="C10">
+        <v>1.9983440000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>7.6697050000000003E-2</v>
+      </c>
+      <c r="C11">
+        <v>3.9596689999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <f>AVERAGE(B2:B11)</f>
+        <v>6.736370500000001E-2</v>
+      </c>
+      <c r="C13">
+        <f>AVERAGE(C2:C11)</f>
+        <v>3.5546943999999997E-2</v>
+      </c>
+      <c r="D13">
+        <f>AVERAGE(D2:D11)</f>
+        <v>1.512374E-2</v>
+      </c>
+      <c r="E13" t="e">
+        <f t="shared" ref="E13:H13" si="0">AVERAGE(E2:E11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>1.35409E-2</v>
+      </c>
+      <c r="H13" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I13">
+        <f>AVERAGE(I2:I6)</f>
+        <v>1.2524159999999998E-2</v>
+      </c>
+      <c r="J13">
+        <f>AVERAGE(J2:J6)</f>
+        <v>2.3581599999999998E-2</v>
+      </c>
+      <c r="K13" t="e">
+        <f>AVERAGE(K2:K6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <f>_xlfn.STDEV.P(B2:B11)</f>
+        <v>9.9474631418057582E-3</v>
+      </c>
+      <c r="C14">
+        <f>_xlfn.STDEV.P(C2:C11)</f>
+        <v>8.5449813137914027E-3</v>
+      </c>
+      <c r="D14">
+        <f>_xlfn.STDEV.P(D2:D11)</f>
+        <v>1.8065069527682426E-3</v>
+      </c>
+      <c r="E14" t="e">
+        <f t="shared" ref="E14:H14" si="1">_xlfn.STDEV.P(E2:E11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>7.408038093854539E-4</v>
+      </c>
+      <c r="H14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I14">
+        <f>_xlfn.STDEV.P(I2:I6)</f>
+        <v>6.1233860110236399E-4</v>
+      </c>
+      <c r="J14">
+        <f>_xlfn.STDEV.P(J2:J6)</f>
+        <v>7.3468811069732137E-4</v>
+      </c>
+      <c r="K14" t="e">
+        <f>_xlfn.STDEV.P(K2:K6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>256</v>
+      </c>
+      <c r="F15">
+        <v>512</v>
+      </c>
+      <c r="G15">
+        <v>1024</v>
+      </c>
+      <c r="H15">
+        <v>4096</v>
+      </c>
+      <c r="I15">
+        <v>8192</v>
+      </c>
+      <c r="J15">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <f>((B13-D13)/B13)*100</f>
+        <v>77.549126788676489</v>
+      </c>
+      <c r="C16">
+        <f>((C13-D13)/C13)*100</f>
+        <v>57.454176651585009</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I have the basics of the fast spiking neuron working. It did slow down compared to my earlier tests, but not horribly so. It is about 3 times slower. I am doing a lot more global IO now though, so that it is understandable. One thing that still needs to be tested is how the speed will change when I have random number of synaptic connections instead of a uniform number that I am using now.
</commit_message>
<xml_diff>
--- a/Libraries/OpenNeuronCL/PerformanceStats.xlsx
+++ b/Libraries/OpenNeuronCL/PerformanceStats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="1305" windowWidth="11010" windowHeight="11760" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="4560" yWindow="1305" windowWidth="11010" windowHeight="11760" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Comparisons" sheetId="2" r:id="rId1"/>
@@ -14,14 +14,14 @@
     <sheet name="FastSpiking Philox Random " sheetId="6" r:id="rId5"/>
     <sheet name="Synapse Iin consolidation" sheetId="7" r:id="rId6"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="49">
   <si>
     <t>Time</t>
   </si>
@@ -163,6 +163,12 @@
   <si>
     <t>Numer of synapses</t>
   </si>
+  <si>
+    <t>No synapse summation</t>
+  </si>
+  <si>
+    <t>With Synapse summation</t>
+  </si>
 </sst>
 </file>
 
@@ -12325,11 +12331,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="52558464"/>
-        <c:axId val="50991488"/>
+        <c:axId val="45644032"/>
+        <c:axId val="56107008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52558464"/>
+        <c:axId val="45644032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12339,12 +12345,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50991488"/>
+        <c:crossAx val="56107008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="50991488"/>
+        <c:axId val="56107008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12355,7 +12361,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52558464"/>
+        <c:crossAx val="45644032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12562,11 +12568,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="51016064"/>
-        <c:axId val="51017984"/>
+        <c:axId val="57173504"/>
+        <c:axId val="57175424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51016064"/>
+        <c:axId val="57173504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12598,7 +12604,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51017984"/>
+        <c:crossAx val="57175424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12606,7 +12612,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51017984"/>
+        <c:axId val="57175424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12617,7 +12623,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51016064"/>
+        <c:crossAx val="57173504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12820,11 +12826,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="51050752"/>
-        <c:axId val="52691328"/>
+        <c:axId val="57459072"/>
+        <c:axId val="57461376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51050752"/>
+        <c:axId val="57459072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12856,7 +12862,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52691328"/>
+        <c:crossAx val="57461376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12864,7 +12870,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52691328"/>
+        <c:axId val="57461376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12875,7 +12881,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51050752"/>
+        <c:crossAx val="57459072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13078,11 +13084,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="52748672"/>
-        <c:axId val="52750592"/>
+        <c:axId val="113670784"/>
+        <c:axId val="189432576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52748672"/>
+        <c:axId val="113670784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13114,7 +13120,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52750592"/>
+        <c:crossAx val="189432576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13122,7 +13128,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52750592"/>
+        <c:axId val="189432576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13133,7 +13139,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52748672"/>
+        <c:crossAx val="113670784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13336,11 +13342,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="53186560"/>
-        <c:axId val="53188480"/>
+        <c:axId val="43236736"/>
+        <c:axId val="43648512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53186560"/>
+        <c:axId val="43236736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13367,12 +13373,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53188480"/>
+        <c:crossAx val="43648512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13380,7 +13387,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53188480"/>
+        <c:axId val="43648512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13391,7 +13398,266 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53186560"/>
+        <c:crossAx val="43236736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'FastSpiking Philox Random '!$B$14:$J$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>9.9474631418057582E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.5449813137914027E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.8065069527682426E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.408038093854539E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.1233860110236399E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.3468811069732137E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'FastSpiking Philox Random '!$B$14:$J$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>9.9474631418057582E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.5449813137914027E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.8065069527682426E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.408038093854539E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.1233860110236399E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.3468811069732137E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'FastSpiking Philox Random '!$B$1:$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>V2_IGF_100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FSP_100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>OCL 2^10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>OCL 2^12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>OCL 2^14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>OCL 2^16</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>OCL 2^18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>OCL 2^20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>OCL 2^23</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCL 2^24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'FastSpiking Philox Random '!$B$13:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6.736370500000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5546943999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.512374E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.35409E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2524159999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3581599999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="43895808"/>
+        <c:axId val="43902080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="43895808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>AnimatLab</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> 100 Neurons Comparison with OPenCL</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43902080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43902080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43895808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13560,6 +13826,43 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>32</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -30243,7 +30546,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30591,7 +30894,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30942,10 +31245,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30980,15 +31283,15 @@
         <v>2</v>
       </c>
       <c r="C2" s="6">
-        <f>B2*$C$28</f>
+        <f>B2*$C$35</f>
         <v>64</v>
       </c>
       <c r="D2" s="6">
-        <f>$B$30-C2</f>
+        <f>$B$37-C2</f>
         <v>1073741760</v>
       </c>
       <c r="E2" s="5">
-        <f>D2/$C$29</f>
+        <f>D2/$C$36</f>
         <v>53687088</v>
       </c>
     </row>
@@ -30997,19 +31300,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="6">
-        <f t="shared" ref="B3:B25" si="0">POWER(2,A3)</f>
+        <f t="shared" ref="B3:B24" si="0">POWER(2,A3)</f>
         <v>4</v>
       </c>
       <c r="C3" s="6">
-        <f t="shared" ref="C3:C25" si="1">B3*$C$28</f>
+        <f t="shared" ref="C3:C25" si="1">B3*$C$35</f>
         <v>128</v>
       </c>
       <c r="D3" s="6">
-        <f t="shared" ref="D3:D25" si="2">$B$30-C3</f>
+        <f t="shared" ref="D3:D25" si="2">$B$37-C3</f>
         <v>1073741696</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E25" si="3">D3/$C$29</f>
+        <f t="shared" ref="E3:E25" si="3">D3/$C$36</f>
         <v>53687084.799999997</v>
       </c>
     </row>
@@ -31475,35 +31778,182 @@
         <v>26843545.600000001</v>
       </c>
     </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6">
+        <f t="shared" ref="B26:B28" si="4">POWER(2,A26)</f>
+        <v>33554432</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" ref="C26:C28" si="5">B26*$C$35</f>
+        <v>1073741824</v>
+      </c>
+      <c r="D26" s="6">
+        <f t="shared" ref="D26:D28" si="6">$B$37-C26</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" ref="E26:E28" si="7">D26/$C$36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6">
+        <f t="shared" si="4"/>
+        <v>67108864</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="5"/>
+        <v>2147483648</v>
+      </c>
+      <c r="D27" s="6">
+        <f t="shared" si="6"/>
+        <v>-1073741824</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="7"/>
+        <v>-53687091.200000003</v>
+      </c>
+    </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6">
+        <f>POWER(2,A28)</f>
+        <v>134217728</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="5"/>
+        <v>4294967296</v>
+      </c>
+      <c r="D28" s="6">
+        <f t="shared" si="6"/>
+        <v>-3221225472</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="7"/>
+        <v>-161061273.59999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6">
+        <f t="shared" ref="B29:B31" si="8">POWER(2,A29)</f>
+        <v>268435456</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" ref="C29:C32" si="9">B29*$C$35</f>
+        <v>8589934592</v>
+      </c>
+      <c r="D29" s="6">
+        <f t="shared" ref="D29:D32" si="10">$B$37-C29</f>
+        <v>-7516192768</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" ref="E29:E32" si="11">D29/$C$36</f>
+        <v>-375809638.39999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6">
+        <f t="shared" si="8"/>
+        <v>536870912</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="9"/>
+        <v>17179869184</v>
+      </c>
+      <c r="D30" s="6">
+        <f t="shared" si="10"/>
+        <v>-16106127360</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="11"/>
+        <v>-805306368</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6">
+        <f>POWER(2,A31)</f>
+        <v>1073741824</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="9"/>
+        <v>34359738368</v>
+      </c>
+      <c r="D31" s="6">
+        <f t="shared" si="10"/>
+        <v>-33285996544</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="11"/>
+        <v>-1664299827.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6">
+        <f>POWER(2,A32)</f>
+        <v>2147483648</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="9"/>
+        <v>68719476736</v>
+      </c>
+      <c r="D32" s="6">
+        <f t="shared" si="10"/>
+        <v>-67645734912</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="11"/>
+        <v>-3382286745.5999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>41</v>
       </c>
-      <c r="B28">
+      <c r="B35">
         <v>8</v>
       </c>
-      <c r="C28">
-        <f>B28*4</f>
+      <c r="C35">
+        <f>B35*4</f>
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>42</v>
       </c>
-      <c r="B29">
+      <c r="B36">
         <v>5</v>
       </c>
-      <c r="C29">
-        <f>B29*4</f>
+      <c r="C36">
+        <f>B36*4</f>
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B37" s="6">
         <f>1024*2^20</f>
         <v>1073741824</v>
       </c>
@@ -31512,4 +31962,506 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>7.2041859999999999E-2</v>
+      </c>
+      <c r="C3">
+        <v>4.0023969999999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>2.7405800000000001E-2</v>
+      </c>
+      <c r="E3">
+        <v>2.39908E-2</v>
+      </c>
+      <c r="F3">
+        <v>2.1570300000000001E-2</v>
+      </c>
+      <c r="K3">
+        <v>7.2041859999999999E-2</v>
+      </c>
+      <c r="L3">
+        <v>4.0023969999999999E-2</v>
+      </c>
+      <c r="M3">
+        <v>2.8572199999999999E-2</v>
+      </c>
+      <c r="N3">
+        <v>2.17877E-2</v>
+      </c>
+      <c r="O3">
+        <v>2.6980500000000001E-2</v>
+      </c>
+      <c r="P3">
+        <v>3.8556600000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>5.2445930000000002E-2</v>
+      </c>
+      <c r="C4">
+        <v>1.764429E-2</v>
+      </c>
+      <c r="D4">
+        <v>2.7970999999999999E-2</v>
+      </c>
+      <c r="E4">
+        <v>2.15529E-2</v>
+      </c>
+      <c r="F4">
+        <v>2.3652099999999999E-2</v>
+      </c>
+      <c r="K4">
+        <v>5.2445930000000002E-2</v>
+      </c>
+      <c r="L4">
+        <v>1.764429E-2</v>
+      </c>
+      <c r="M4">
+        <v>3.06489E-2</v>
+      </c>
+      <c r="N4">
+        <v>2.07625E-2</v>
+      </c>
+      <c r="O4">
+        <v>2.5256000000000001E-2</v>
+      </c>
+      <c r="P4">
+        <v>5.2176800000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>7.4952640000000001E-2</v>
+      </c>
+      <c r="C5">
+        <v>4.3591709999999999E-2</v>
+      </c>
+      <c r="D5">
+        <v>3.0133699999999999E-2</v>
+      </c>
+      <c r="E5">
+        <v>2.1569000000000001E-2</v>
+      </c>
+      <c r="F5">
+        <v>2.59431E-2</v>
+      </c>
+      <c r="K5">
+        <v>7.4952640000000001E-2</v>
+      </c>
+      <c r="L5">
+        <v>4.3591709999999999E-2</v>
+      </c>
+      <c r="M5">
+        <v>3.09427E-2</v>
+      </c>
+      <c r="N5">
+        <v>2.1025599999999998E-2</v>
+      </c>
+      <c r="O5">
+        <v>2.2586499999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>7.2751430000000006E-2</v>
+      </c>
+      <c r="C6">
+        <v>3.9400369999999997E-2</v>
+      </c>
+      <c r="D6">
+        <v>3.0133699999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>2.0371199999999999E-2</v>
+      </c>
+      <c r="F6">
+        <v>2.6448599999999999E-2</v>
+      </c>
+      <c r="K6">
+        <v>7.2751430000000006E-2</v>
+      </c>
+      <c r="L6">
+        <v>3.9400369999999997E-2</v>
+      </c>
+      <c r="M6">
+        <v>3.1549000000000001E-2</v>
+      </c>
+      <c r="N6">
+        <v>2.1025599999999998E-2</v>
+      </c>
+      <c r="O6">
+        <v>2.3816299999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>7.2371619999999998E-2</v>
+      </c>
+      <c r="C7">
+        <v>4.0634099999999999E-2</v>
+      </c>
+      <c r="D7">
+        <v>2.80288E-2</v>
+      </c>
+      <c r="E7">
+        <v>2.38471E-2</v>
+      </c>
+      <c r="F7">
+        <v>2.56679E-2</v>
+      </c>
+      <c r="K7">
+        <v>7.2371619999999998E-2</v>
+      </c>
+      <c r="L7">
+        <v>4.0634099999999999E-2</v>
+      </c>
+      <c r="M7">
+        <v>3.0260100000000002E-2</v>
+      </c>
+      <c r="N7">
+        <v>2.6534599999999998E-2</v>
+      </c>
+      <c r="O7">
+        <v>2.60868E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>7.2689199999999995E-2</v>
+      </c>
+      <c r="C8">
+        <v>3.6535140000000001E-2</v>
+      </c>
+      <c r="K8">
+        <v>7.2689199999999995E-2</v>
+      </c>
+      <c r="L8">
+        <v>3.6535140000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>4.8488759999999999E-2</v>
+      </c>
+      <c r="C9">
+        <v>3.9424109999999998E-2</v>
+      </c>
+      <c r="K9">
+        <v>4.8488759999999999E-2</v>
+      </c>
+      <c r="L9">
+        <v>3.9424109999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7.4415010000000004E-2</v>
+      </c>
+      <c r="C10">
+        <v>3.8635620000000002E-2</v>
+      </c>
+      <c r="K10">
+        <v>7.4415010000000004E-2</v>
+      </c>
+      <c r="L10">
+        <v>3.8635620000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>5.6783550000000002E-2</v>
+      </c>
+      <c r="C11">
+        <v>1.9983440000000002E-2</v>
+      </c>
+      <c r="K11">
+        <v>5.6783550000000002E-2</v>
+      </c>
+      <c r="L11">
+        <v>1.9983440000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>7.6697050000000003E-2</v>
+      </c>
+      <c r="C12">
+        <v>3.9596689999999997E-2</v>
+      </c>
+      <c r="K12">
+        <v>7.6697050000000003E-2</v>
+      </c>
+      <c r="L12">
+        <v>3.9596689999999997E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:E14" si="0">AVERAGE(B3:B12)</f>
+        <v>6.736370500000001E-2</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>3.5546943999999997E-2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>2.8734599999999999E-2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>2.22662E-2</v>
+      </c>
+      <c r="F14">
+        <f>AVERAGE(F3:F7)</f>
+        <v>2.4656400000000002E-2</v>
+      </c>
+      <c r="G14" t="e">
+        <f>AVERAGE(G3:G7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ref="K14:N14" si="1">AVERAGE(K3:K12)</f>
+        <v>6.736370500000001E-2</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="1"/>
+        <v>3.5546943999999997E-2</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>3.0394580000000004E-2</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>2.2227199999999996E-2</v>
+      </c>
+      <c r="O14">
+        <f>AVERAGE(O3:O7)</f>
+        <v>2.4945220000000001E-2</v>
+      </c>
+      <c r="P14">
+        <f>AVERAGE(P3:P7)</f>
+        <v>4.5366700000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:E15" si="2">_xlfn.STDEV.P(B3:B12)</f>
+        <v>9.9474631418057582E-3</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>8.5449813137914027E-3</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>1.162919572455464E-3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>1.4184075366410036E-3</v>
+      </c>
+      <c r="F15">
+        <f>_xlfn.STDEV.P(F3:F7)</f>
+        <v>1.8123653980364994E-3</v>
+      </c>
+      <c r="G15" t="e">
+        <f>_xlfn.STDEV.P(G3:G7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ref="K15:N15" si="3">_xlfn.STDEV.P(K3:K12)</f>
+        <v>9.9474631418057582E-3</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>8.5449813137914027E-3</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
+        <v>1.0036885441211338E-3</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="3"/>
+        <v>2.1808203144688468E-3</v>
+      </c>
+      <c r="O15">
+        <f>_xlfn.STDEV.P(O3:O7)</f>
+        <v>1.5735421308627241E-3</v>
+      </c>
+      <c r="P15">
+        <f>_xlfn.STDEV.P(P3:P7)</f>
+        <v>6.8100999999999943E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>1024</v>
+      </c>
+      <c r="F16">
+        <v>8192</v>
+      </c>
+      <c r="G16">
+        <v>16384</v>
+      </c>
+      <c r="J16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+      <c r="L16">
+        <v>100</v>
+      </c>
+      <c r="M16">
+        <v>100</v>
+      </c>
+      <c r="N16">
+        <v>1024</v>
+      </c>
+      <c r="O16">
+        <v>8192</v>
+      </c>
+      <c r="P16">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <f>((B14-D14)/B14)*100</f>
+        <v>57.34409204481851</v>
+      </c>
+      <c r="C17">
+        <f>((C14-D14)/C14)*100</f>
+        <v>19.164359107775901</v>
+      </c>
+      <c r="J17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <f>((K14-M14)/K14)*100</f>
+        <v>54.879886728320535</v>
+      </c>
+      <c r="L17">
+        <f>((L14-M14)/L14)*100</f>
+        <v>14.49453432621379</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tested the fast spiking synapse model connection to a second neuron.
</commit_message>
<xml_diff>
--- a/Libraries/OpenNeuronCL/PerformanceStats.xlsx
+++ b/Libraries/OpenNeuronCL/PerformanceStats.xlsx
@@ -363,7 +363,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'FS 1Syn'!$A$37</c:f>
+              <c:f>'FS 1Syn'!$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -396,7 +396,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'FS 1Syn'!$D$36:$I$36</c:f>
+                <c:f>'FS 1Syn'!$D$37:$I$37</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -417,7 +417,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'FS 1Syn'!$D$36:$I$36</c:f>
+                <c:f>'FS 1Syn'!$D$37:$I$37</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -439,7 +439,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'FS 1Syn'!$D$34:$I$34</c:f>
+              <c:f>'FS 1Syn'!$D$35:$I$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -466,7 +466,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'FS 1Syn'!$D$35:$I$35</c:f>
+              <c:f>'FS 1Syn'!$D$36:$I$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -492,7 +492,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'FS 1Syn'!$A$58</c:f>
+              <c:f>'FS 1Syn'!$A$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -525,7 +525,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'FS 1Syn'!$D$57:$I$57</c:f>
+                <c:f>'FS 1Syn'!$D$58:$I$58</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -546,7 +546,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'FS 1Syn'!$D$57:$I$57</c:f>
+                <c:f>'FS 1Syn'!$D$58:$I$58</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -568,7 +568,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'FS 1Syn'!$D$54:$I$54</c:f>
+              <c:f>'FS 1Syn'!$D$55:$I$55</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
@@ -595,7 +595,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'FS 1Syn'!$D$56:$I$56</c:f>
+              <c:f>'FS 1Syn'!$D$57:$I$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -668,7 +668,7 @@
           <c:x val="0.11769335083114608"/>
           <c:y val="9.6838363954505693E-2"/>
           <c:w val="0.30663375766274531"/>
-          <c:h val="0.35896602254742971"/>
+          <c:h val="0.34199363377450159"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -689,16 +689,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>466724</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1007,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35:K36"/>
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,47 +1458,47 @@
         <v>6.736370500000001E-2</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" ref="C16:E16" si="9">AVERAGE(C3:C12)</f>
+        <f>AVERAGE(C3:C12)</f>
         <v>3.5546943999999997E-2</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="9"/>
+        <f>AVERAGE(D3:D12)</f>
         <v>6.4787140000000007E-2</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="9"/>
+        <f>AVERAGE(E3:E12)</f>
         <v>9.6337759999999995E-2</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" ref="F16:M16" si="10">AVERAGE(F3:F12)</f>
+        <f>AVERAGE(F3:F12)</f>
         <v>0.10058032000000001</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="10"/>
+        <f>AVERAGE(G3:G12)</f>
         <v>0.14493329999999999</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="10"/>
+        <f>AVERAGE(H3:H12)</f>
         <v>0.17089299999999999</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="10"/>
+        <f>AVERAGE(I3:I12)</f>
         <v>0.28261999999999998</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="10"/>
+        <f>AVERAGE(J3:J12)</f>
         <v>0.39754899999999999</v>
       </c>
       <c r="K16" s="2">
-        <f t="shared" si="10"/>
+        <f>AVERAGE(K3:K12)</f>
         <v>0.7148230000000001</v>
       </c>
       <c r="L16" s="2">
-        <f t="shared" si="10"/>
+        <f>AVERAGE(L3:L12)</f>
         <v>1.3021160000000001</v>
       </c>
       <c r="M16" s="2">
-        <f t="shared" si="10"/>
+        <f>AVERAGE(M3:M12)</f>
         <v>2.5754700000000001</v>
       </c>
     </row>
@@ -1511,47 +1511,47 @@
         <v>9.9474631418057582E-3</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" ref="C17:E17" si="11">_xlfn.STDEV.P(C3:C12)</f>
+        <f>_xlfn.STDEV.P(C3:C12)</f>
         <v>8.5449813137914027E-3</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="11"/>
+        <f>_xlfn.STDEV.P(D3:D12)</f>
         <v>1.0314438191312168E-2</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="11"/>
+        <f>_xlfn.STDEV.P(E3:E12)</f>
         <v>1.2884209919215137E-2</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" ref="F17:M17" si="12">_xlfn.STDEV.P(F3:F12)</f>
+        <f>_xlfn.STDEV.P(F3:F12)</f>
         <v>3.3958549890323604E-2</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="12"/>
+        <f>_xlfn.STDEV.P(G3:G12)</f>
         <v>4.253197212328623E-2</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" si="12"/>
+        <f>_xlfn.STDEV.P(H3:H12)</f>
         <v>6.264397656598762E-3</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="12"/>
+        <f>_xlfn.STDEV.P(I3:I12)</f>
         <v>6.5537341111766238E-3</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="12"/>
+        <f>_xlfn.STDEV.P(J3:J12)</f>
         <v>3.5042366603869682E-2</v>
       </c>
       <c r="K17" s="2">
-        <f t="shared" si="12"/>
+        <f>_xlfn.STDEV.P(K3:K12)</f>
         <v>3.3122125493391871E-2</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="12"/>
+        <f>_xlfn.STDEV.P(L3:L12)</f>
         <v>1.0405641931183271E-2</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" si="12"/>
+        <f>_xlfn.STDEV.P(M3:M12)</f>
         <v>3.449633951595437E-2</v>
       </c>
     </row>
@@ -1568,104 +1568,82 @@
       <c r="K18" s="2"/>
       <c r="M18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="19" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="M21" s="2"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="2">
-        <v>7.2041859999999999E-2</v>
-      </c>
-      <c r="C22" s="2">
-        <v>4.0023969999999999E-2</v>
-      </c>
-      <c r="D22" s="2">
-        <v>8.2152699999999995E-2</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.18873799999999999</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0.389235</v>
-      </c>
-      <c r="I22" s="2">
-        <v>1.3515600000000001</v>
-      </c>
-      <c r="K22" s="2"/>
-      <c r="M22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2">
-        <v>5.2445930000000002E-2</v>
+        <v>7.2041859999999999E-2</v>
       </c>
       <c r="C23" s="2">
-        <v>1.764429E-2</v>
+        <v>4.0023969999999999E-2</v>
       </c>
       <c r="D23" s="2">
-        <v>7.6092599999999996E-2</v>
+        <v>8.2152699999999995E-2</v>
       </c>
       <c r="E23" s="2">
-        <v>0.17513500000000001</v>
+        <v>0.18873799999999999</v>
       </c>
       <c r="G23" s="2">
-        <v>0.475715</v>
+        <v>0.389235</v>
       </c>
       <c r="I23" s="2">
-        <v>1.34701</v>
+        <v>1.3515600000000001</v>
       </c>
       <c r="K23" s="2"/>
       <c r="M23" s="2"/>
@@ -1673,22 +1651,22 @@
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2">
-        <v>7.4952640000000001E-2</v>
+        <v>5.2445930000000002E-2</v>
       </c>
       <c r="C24" s="2">
-        <v>4.3591709999999999E-2</v>
+        <v>1.764429E-2</v>
       </c>
       <c r="D24" s="2">
-        <v>6.7135899999999998E-2</v>
+        <v>7.6092599999999996E-2</v>
       </c>
       <c r="E24" s="2">
-        <v>0.19551199999999999</v>
+        <v>0.17513500000000001</v>
       </c>
       <c r="G24" s="2">
-        <v>0.37502200000000002</v>
+        <v>0.475715</v>
       </c>
       <c r="I24" s="2">
-        <v>1.32962</v>
+        <v>1.34701</v>
       </c>
       <c r="K24" s="2"/>
       <c r="M24" s="2"/>
@@ -1696,22 +1674,22 @@
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2">
-        <v>7.2751430000000006E-2</v>
+        <v>7.4952640000000001E-2</v>
       </c>
       <c r="C25" s="2">
-        <v>3.9400369999999997E-2</v>
+        <v>4.3591709999999999E-2</v>
       </c>
       <c r="D25" s="2">
-        <v>8.3688499999999999E-2</v>
+        <v>6.7135899999999998E-2</v>
       </c>
       <c r="E25" s="2">
-        <v>0.20033500000000001</v>
+        <v>0.19551199999999999</v>
       </c>
       <c r="G25" s="2">
-        <v>0.38320799999999999</v>
+        <v>0.37502200000000002</v>
       </c>
       <c r="I25" s="2">
-        <v>1.34989</v>
+        <v>1.32962</v>
       </c>
       <c r="K25" s="2"/>
       <c r="M25" s="2"/>
@@ -1719,22 +1697,22 @@
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2">
-        <v>7.2371619999999998E-2</v>
+        <v>7.2751430000000006E-2</v>
       </c>
       <c r="C26" s="2">
-        <v>4.0634099999999999E-2</v>
+        <v>3.9400369999999997E-2</v>
       </c>
       <c r="D26" s="2">
-        <v>9.8876000000000006E-2</v>
+        <v>8.3688499999999999E-2</v>
       </c>
       <c r="E26" s="2">
-        <v>0.20824899999999999</v>
+        <v>0.20033500000000001</v>
       </c>
       <c r="G26" s="2">
-        <v>0.38973999999999998</v>
+        <v>0.38320799999999999</v>
       </c>
       <c r="I26" s="2">
-        <v>1.3640699999999999</v>
+        <v>1.34989</v>
       </c>
       <c r="K26" s="2"/>
       <c r="M26" s="2"/>
@@ -1742,25 +1720,33 @@
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2">
-        <v>7.2689199999999995E-2</v>
+        <v>7.2371619999999998E-2</v>
       </c>
       <c r="C27" s="2">
-        <v>3.6535140000000001E-2</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="I27" s="2"/>
+        <v>4.0634099999999999E-2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>9.8876000000000006E-2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.20824899999999999</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.38973999999999998</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1.3640699999999999</v>
+      </c>
       <c r="K27" s="2"/>
       <c r="M27" s="2"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2">
-        <v>4.8488759999999999E-2</v>
+        <v>7.2689199999999995E-2</v>
       </c>
       <c r="C28" s="2">
-        <v>3.9424109999999998E-2</v>
+        <v>3.6535140000000001E-2</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1772,10 +1758,10 @@
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2">
-        <v>7.4415010000000004E-2</v>
+        <v>4.8488759999999999E-2</v>
       </c>
       <c r="C29" s="2">
-        <v>3.8635620000000002E-2</v>
+        <v>3.9424109999999998E-2</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1787,10 +1773,10 @@
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2">
-        <v>5.6783550000000002E-2</v>
+        <v>7.4415010000000004E-2</v>
       </c>
       <c r="C30" s="2">
-        <v>1.9983440000000002E-2</v>
+        <v>3.8635620000000002E-2</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1802,10 +1788,10 @@
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2">
-        <v>7.6697050000000003E-2</v>
+        <v>5.6783550000000002E-2</v>
       </c>
       <c r="C31" s="2">
-        <v>3.9596689999999997E-2</v>
+        <v>1.9983440000000002E-2</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1816,8 +1802,12 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="2">
+        <v>7.6697050000000003E-2</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3.9596689999999997E-2</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="G32" s="2"/>
@@ -1826,254 +1816,242 @@
       <c r="M32" s="2"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="2">
-        <v>10</v>
-      </c>
-      <c r="E33" s="2">
-        <v>12</v>
-      </c>
-      <c r="F33" s="2">
-        <v>13</v>
-      </c>
-      <c r="G33" s="2">
-        <v>14</v>
-      </c>
-      <c r="H33" s="2">
-        <v>15</v>
-      </c>
-      <c r="I33" s="2">
-        <v>16</v>
-      </c>
-      <c r="J33" s="2">
-        <v>17</v>
-      </c>
-      <c r="K33" s="2">
-        <v>18</v>
-      </c>
-      <c r="L33" s="2">
-        <v>19</v>
-      </c>
-      <c r="M33" s="2">
-        <v>20</v>
-      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="M33" s="2"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2">
         <v>10</v>
       </c>
-      <c r="B34" s="2">
-        <v>100</v>
-      </c>
-      <c r="C34" s="2">
-        <v>100</v>
-      </c>
-      <c r="D34" s="2">
-        <f>2^D33</f>
-        <v>1024</v>
-      </c>
       <c r="E34" s="2">
-        <f t="shared" ref="E34" si="13">2^E33</f>
-        <v>4096</v>
+        <v>12</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" ref="F34" si="14">2^F33</f>
-        <v>8192</v>
+        <v>13</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" ref="G34" si="15">2^G33</f>
-        <v>16384</v>
+        <v>14</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" ref="H34" si="16">2^H33</f>
-        <v>32768</v>
+        <v>15</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" ref="I34" si="17">2^I33</f>
-        <v>65536</v>
+        <v>16</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" ref="J34" si="18">2^J33</f>
-        <v>131072</v>
+        <v>17</v>
       </c>
       <c r="K34" s="2">
-        <f t="shared" ref="K34" si="19">2^K33</f>
-        <v>262144</v>
+        <v>18</v>
       </c>
       <c r="L34" s="2">
-        <f t="shared" ref="L34" si="20">2^L33</f>
-        <v>524288</v>
+        <v>19</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" ref="M34" si="21">2^M33</f>
-        <v>1048576</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B35" s="2">
-        <f>AVERAGE(B22:B31)</f>
-        <v>6.736370500000001E-2</v>
+        <v>100</v>
       </c>
       <c r="C35" s="2">
-        <f t="shared" ref="C35:M35" si="22">AVERAGE(C22:C31)</f>
-        <v>3.5546943999999997E-2</v>
+        <v>100</v>
       </c>
       <c r="D35" s="2">
-        <f t="shared" si="22"/>
-        <v>8.1589140000000004E-2</v>
+        <f>2^D34</f>
+        <v>1024</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="22"/>
-        <v>0.19359380000000001</v>
+        <f t="shared" ref="E35" si="9">2^E34</f>
+        <v>4096</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" ref="F35" si="10">2^F34</f>
+        <v>8192</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" si="22"/>
-        <v>0.40258400000000005</v>
+        <f t="shared" ref="G35" si="11">2^G34</f>
+        <v>16384</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" ref="H35" si="12">2^H34</f>
+        <v>32768</v>
       </c>
       <c r="I35" s="2">
-        <f t="shared" si="22"/>
-        <v>1.34843</v>
-      </c>
-      <c r="K35" s="2"/>
-      <c r="M35" s="2"/>
+        <f t="shared" ref="I35" si="13">2^I34</f>
+        <v>65536</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" ref="J35" si="14">2^J34</f>
+        <v>131072</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" ref="K35" si="15">2^K34</f>
+        <v>262144</v>
+      </c>
+      <c r="L35" s="2">
+        <f t="shared" ref="L35" si="16">2^L34</f>
+        <v>524288</v>
+      </c>
+      <c r="M35" s="2">
+        <f t="shared" ref="M35" si="17">2^M34</f>
+        <v>1048576</v>
+      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" s="2">
-        <f>_xlfn.STDEV.P(B22:B31)</f>
-        <v>9.9474631418057582E-3</v>
+        <f>AVERAGE(B23:B32)</f>
+        <v>6.736370500000001E-2</v>
       </c>
       <c r="C36" s="2">
-        <f t="shared" ref="C36:M36" si="23">_xlfn.STDEV.P(C22:C31)</f>
-        <v>8.5449813137914027E-3</v>
+        <f t="shared" ref="C36:I36" si="18">AVERAGE(C23:C32)</f>
+        <v>3.5546943999999997E-2</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" si="23"/>
-        <v>1.0417951232483286E-2</v>
+        <f t="shared" si="18"/>
+        <v>8.1589140000000004E-2</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="23"/>
-        <v>1.1208962902962964E-2</v>
+        <f t="shared" si="18"/>
+        <v>0.19359380000000001</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="23"/>
-        <v>3.6949696935157664E-2</v>
+        <f t="shared" si="18"/>
+        <v>0.40258400000000005</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" si="23"/>
-        <v>1.1066802609606772E-2</v>
+        <f t="shared" si="18"/>
+        <v>1.34843</v>
       </c>
       <c r="K36" s="2"/>
       <c r="M36" s="2"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="2">
+        <f>_xlfn.STDEV.P(B23:B32)</f>
+        <v>9.9474631418057582E-3</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" ref="C37:I37" si="19">_xlfn.STDEV.P(C23:C32)</f>
+        <v>8.5449813137914027E-3</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="19"/>
+        <v>1.0417951232483286E-2</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="19"/>
+        <v>1.1208962902962964E-2</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="19"/>
+        <v>3.6949696935157664E-2</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="19"/>
+        <v>1.1066802609606772E-2</v>
+      </c>
+      <c r="K37" s="2"/>
+      <c r="M37" s="2"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+    <row r="41" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="M40" s="2"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="M41" s="2"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" s="2">
-        <v>7.2041859999999999E-2</v>
-      </c>
-      <c r="C42" s="2">
-        <v>4.0023969999999999E-2</v>
-      </c>
-      <c r="D42" s="2">
-        <v>0.17308499999999999</v>
-      </c>
-      <c r="E42" s="2">
-        <v>0.28573799999999999</v>
-      </c>
-      <c r="G42" s="2">
-        <v>0.83005799999999996</v>
-      </c>
-      <c r="I42" s="2">
-        <v>2.7700300000000002</v>
-      </c>
-      <c r="K42" s="2"/>
-      <c r="M42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2">
-        <v>5.2445930000000002E-2</v>
+        <v>7.2041859999999999E-2</v>
       </c>
       <c r="C43" s="2">
-        <v>1.764429E-2</v>
+        <v>4.0023969999999999E-2</v>
       </c>
       <c r="D43" s="2">
-        <v>0.19839899999999999</v>
+        <v>0.17308499999999999</v>
       </c>
       <c r="E43" s="2">
-        <v>0.27193899999999999</v>
+        <v>0.28573799999999999</v>
       </c>
       <c r="G43" s="2">
-        <v>0.82374899999999995</v>
+        <v>0.83005799999999996</v>
       </c>
       <c r="I43" s="2">
-        <v>2.7398600000000002</v>
+        <v>2.7700300000000002</v>
       </c>
       <c r="K43" s="2"/>
       <c r="M43" s="2"/>
@@ -2081,22 +2059,22 @@
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2">
-        <v>7.4952640000000001E-2</v>
+        <v>5.2445930000000002E-2</v>
       </c>
       <c r="C44" s="2">
-        <v>4.3591709999999999E-2</v>
+        <v>1.764429E-2</v>
       </c>
       <c r="D44" s="2">
-        <v>0.19333700000000001</v>
+        <v>0.19839899999999999</v>
       </c>
       <c r="E44" s="2">
-        <v>0.28915600000000002</v>
+        <v>0.27193899999999999</v>
       </c>
       <c r="G44" s="2">
-        <v>0.80301900000000004</v>
+        <v>0.82374899999999995</v>
       </c>
       <c r="I44" s="2">
-        <v>2.77671</v>
+        <v>2.7398600000000002</v>
       </c>
       <c r="K44" s="2"/>
       <c r="M44" s="2"/>
@@ -2104,22 +2082,22 @@
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2">
-        <v>7.2751430000000006E-2</v>
+        <v>7.4952640000000001E-2</v>
       </c>
       <c r="C45" s="2">
-        <v>3.9400369999999997E-2</v>
+        <v>4.3591709999999999E-2</v>
       </c>
       <c r="D45" s="2">
-        <v>0.192636</v>
+        <v>0.19333700000000001</v>
       </c>
       <c r="E45" s="2">
-        <v>0.28279399999999999</v>
-      </c>
-      <c r="G45">
-        <v>0.84062099999999995</v>
+        <v>0.28915600000000002</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0.80301900000000004</v>
       </c>
       <c r="I45" s="2">
-        <v>2.7493799999999999</v>
+        <v>2.77671</v>
       </c>
       <c r="K45" s="2"/>
       <c r="M45" s="2"/>
@@ -2127,22 +2105,22 @@
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2">
-        <v>7.2371619999999998E-2</v>
+        <v>7.2751430000000006E-2</v>
       </c>
       <c r="C46" s="2">
-        <v>4.0634099999999999E-2</v>
+        <v>3.9400369999999997E-2</v>
       </c>
       <c r="D46" s="2">
         <v>0.192636</v>
       </c>
       <c r="E46" s="2">
-        <v>0.30924600000000002</v>
-      </c>
-      <c r="G46" s="2">
-        <v>0.80660699999999996</v>
+        <v>0.28279399999999999</v>
+      </c>
+      <c r="G46">
+        <v>0.84062099999999995</v>
       </c>
       <c r="I46" s="2">
-        <v>2.7599399999999998</v>
+        <v>2.7493799999999999</v>
       </c>
       <c r="K46" s="2"/>
       <c r="M46" s="2"/>
@@ -2150,25 +2128,33 @@
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2">
-        <v>7.2689199999999995E-2</v>
+        <v>7.2371619999999998E-2</v>
       </c>
       <c r="C47" s="2">
-        <v>3.6535140000000001E-2</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="I47" s="2"/>
+        <v>4.0634099999999999E-2</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.192636</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0.30924600000000002</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0.80660699999999996</v>
+      </c>
+      <c r="I47" s="2">
+        <v>2.7599399999999998</v>
+      </c>
       <c r="K47" s="2"/>
       <c r="M47" s="2"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2">
-        <v>4.8488759999999999E-2</v>
+        <v>7.2689199999999995E-2</v>
       </c>
       <c r="C48" s="2">
-        <v>3.9424109999999998E-2</v>
+        <v>3.6535140000000001E-2</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -2180,10 +2166,10 @@
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2">
-        <v>7.4415010000000004E-2</v>
+        <v>4.8488759999999999E-2</v>
       </c>
       <c r="C49" s="2">
-        <v>3.8635620000000002E-2</v>
+        <v>3.9424109999999998E-2</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -2195,10 +2181,10 @@
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2">
-        <v>5.6783550000000002E-2</v>
+        <v>7.4415010000000004E-2</v>
       </c>
       <c r="C50" s="2">
-        <v>1.9983440000000002E-2</v>
+        <v>3.8635620000000002E-2</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -2210,10 +2196,10 @@
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2">
-        <v>7.6697050000000003E-2</v>
+        <v>5.6783550000000002E-2</v>
       </c>
       <c r="C51" s="2">
-        <v>3.9596689999999997E-2</v>
+        <v>1.9983440000000002E-2</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2224,8 +2210,12 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="2">
+        <v>7.6697050000000003E-2</v>
+      </c>
+      <c r="C52" s="2">
+        <v>3.9596689999999997E-2</v>
+      </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="G52" s="2"/>
@@ -2234,202 +2224,213 @@
       <c r="M52" s="2"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="2">
-        <v>10</v>
-      </c>
-      <c r="E53" s="2">
-        <v>12</v>
-      </c>
-      <c r="F53" s="2">
-        <v>13</v>
-      </c>
-      <c r="G53" s="2">
-        <v>14</v>
-      </c>
-      <c r="H53" s="2">
-        <v>15</v>
-      </c>
-      <c r="I53" s="2">
-        <v>16</v>
-      </c>
-      <c r="J53" s="2">
-        <v>17</v>
-      </c>
-      <c r="K53" s="2">
-        <v>18</v>
-      </c>
-      <c r="L53" s="2">
-        <v>19</v>
-      </c>
-      <c r="M53" s="2">
-        <v>20</v>
-      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="M53" s="2"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2">
         <v>10</v>
       </c>
-      <c r="B54" s="2">
+      <c r="E54" s="2">
+        <v>12</v>
+      </c>
+      <c r="F54" s="2">
+        <v>13</v>
+      </c>
+      <c r="G54" s="2">
+        <v>14</v>
+      </c>
+      <c r="H54" s="2">
+        <v>15</v>
+      </c>
+      <c r="I54" s="2">
+        <v>16</v>
+      </c>
+      <c r="J54" s="2">
+        <v>17</v>
+      </c>
+      <c r="K54" s="2">
+        <v>18</v>
+      </c>
+      <c r="L54" s="2">
+        <v>19</v>
+      </c>
+      <c r="M54" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="2">
         <v>100</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C55" s="2">
         <v>100</v>
       </c>
-      <c r="D54" s="3">
-        <f>2^D53</f>
+      <c r="D55" s="3">
+        <f>2^D54</f>
         <v>1024</v>
       </c>
-      <c r="E54" s="3">
-        <f t="shared" ref="E54" si="24">2^E53</f>
+      <c r="E55" s="3">
+        <f t="shared" ref="E55" si="20">2^E54</f>
         <v>4096</v>
       </c>
-      <c r="F54" s="3">
-        <f t="shared" ref="F54" si="25">2^F53</f>
+      <c r="F55" s="3">
+        <f t="shared" ref="F55" si="21">2^F54</f>
         <v>8192</v>
       </c>
-      <c r="G54" s="3">
-        <f t="shared" ref="G54" si="26">2^G53</f>
+      <c r="G55" s="3">
+        <f t="shared" ref="G55" si="22">2^G54</f>
         <v>16384</v>
       </c>
-      <c r="H54" s="3">
-        <f t="shared" ref="H54" si="27">2^H53</f>
+      <c r="H55" s="3">
+        <f t="shared" ref="H55" si="23">2^H54</f>
         <v>32768</v>
       </c>
-      <c r="I54" s="3">
-        <f t="shared" ref="I54" si="28">2^I53</f>
+      <c r="I55" s="3">
+        <f t="shared" ref="I55" si="24">2^I54</f>
         <v>65536</v>
       </c>
-      <c r="J54" s="3">
-        <f t="shared" ref="J54" si="29">2^J53</f>
+      <c r="J55" s="3">
+        <f t="shared" ref="J55" si="25">2^J54</f>
         <v>131072</v>
       </c>
-      <c r="K54" s="3">
-        <f t="shared" ref="K54" si="30">2^K53</f>
+      <c r="K55" s="3">
+        <f t="shared" ref="K55" si="26">2^K54</f>
         <v>262144</v>
       </c>
-      <c r="L54" s="3">
-        <f t="shared" ref="L54" si="31">2^L53</f>
+      <c r="L55" s="3">
+        <f t="shared" ref="L55" si="27">2^L54</f>
         <v>524288</v>
       </c>
-      <c r="M54" s="3">
-        <f t="shared" ref="M54" si="32">2^M53</f>
+      <c r="M55" s="3">
+        <f t="shared" ref="M55" si="28">2^M54</f>
         <v>1048576</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="56" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="3">
-        <f>D54*10</f>
+      <c r="D56" s="3">
+        <f>D55*10</f>
         <v>10240</v>
       </c>
-      <c r="E55" s="3">
-        <f t="shared" ref="E55:M55" si="33">E54*10</f>
+      <c r="E56" s="3">
+        <f t="shared" ref="E56:M56" si="29">E55*10</f>
         <v>40960</v>
       </c>
-      <c r="F55" s="3">
-        <f t="shared" si="33"/>
+      <c r="F56" s="3">
+        <f t="shared" si="29"/>
         <v>81920</v>
       </c>
-      <c r="G55" s="3">
-        <f t="shared" si="33"/>
+      <c r="G56" s="3">
+        <f t="shared" si="29"/>
         <v>163840</v>
       </c>
-      <c r="H55" s="3">
-        <f t="shared" si="33"/>
+      <c r="H56" s="3">
+        <f t="shared" si="29"/>
         <v>327680</v>
       </c>
-      <c r="I55" s="3">
-        <f t="shared" si="33"/>
+      <c r="I56" s="3">
+        <f t="shared" si="29"/>
         <v>655360</v>
       </c>
-      <c r="J55" s="3">
-        <f t="shared" si="33"/>
+      <c r="J56" s="3">
+        <f t="shared" si="29"/>
         <v>1310720</v>
       </c>
-      <c r="K55" s="3">
-        <f t="shared" si="33"/>
+      <c r="K56" s="3">
+        <f t="shared" si="29"/>
         <v>2621440</v>
       </c>
-      <c r="L55" s="3">
-        <f t="shared" si="33"/>
+      <c r="L56" s="3">
+        <f t="shared" si="29"/>
         <v>5242880</v>
       </c>
-      <c r="M55" s="3">
-        <f t="shared" si="33"/>
+      <c r="M56" s="3">
+        <f t="shared" si="29"/>
         <v>10485760</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" s="2">
-        <f>AVERAGE(B42:B51)</f>
-        <v>6.736370500000001E-2</v>
-      </c>
-      <c r="C56" s="2">
-        <f t="shared" ref="C56:M56" si="34">AVERAGE(C42:C51)</f>
-        <v>3.5546943999999997E-2</v>
-      </c>
-      <c r="D56" s="2">
-        <f t="shared" si="34"/>
-        <v>0.19001860000000001</v>
-      </c>
-      <c r="E56" s="2">
-        <f t="shared" si="34"/>
-        <v>0.28777459999999999</v>
-      </c>
-      <c r="G56" s="2">
-        <f t="shared" ref="G56:M56" si="35">AVERAGE(G42:G51)</f>
-        <v>0.82081079999999995</v>
-      </c>
-      <c r="I56" s="2">
-        <f t="shared" ref="I56:M56" si="36">AVERAGE(I42:I51)</f>
-        <v>2.7591840000000003</v>
-      </c>
-      <c r="K56" s="2"/>
-      <c r="M56" s="2"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B57" s="2">
-        <f>_xlfn.STDEV.P(B42:B51)</f>
-        <v>9.9474631418057582E-3</v>
+        <f>AVERAGE(B43:B52)</f>
+        <v>6.736370500000001E-2</v>
       </c>
       <c r="C57" s="2">
-        <f t="shared" ref="C57:M57" si="37">_xlfn.STDEV.P(C42:C51)</f>
-        <v>8.5449813137914027E-3</v>
+        <f t="shared" ref="C57:M57" si="30">AVERAGE(C43:C52)</f>
+        <v>3.5546943999999997E-2</v>
       </c>
       <c r="D57" s="2">
-        <f t="shared" si="37"/>
-        <v>8.7371763997300678E-3</v>
+        <f t="shared" si="30"/>
+        <v>0.19001860000000001</v>
       </c>
       <c r="E57" s="2">
-        <f t="shared" si="37"/>
-        <v>1.2187285400777332E-2</v>
+        <f t="shared" si="30"/>
+        <v>0.28777459999999999</v>
       </c>
       <c r="G57" s="2">
-        <f t="shared" ref="G57:M57" si="38">_xlfn.STDEV.P(G42:G51)</f>
-        <v>1.4176627474826281E-2</v>
+        <f t="shared" ref="G57:M57" si="31">AVERAGE(G43:G52)</f>
+        <v>0.82081079999999995</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" ref="I57:M57" si="39">_xlfn.STDEV.P(I42:I51)</f>
-        <v>1.3378365520496135E-2</v>
+        <f t="shared" ref="I57:M57" si="32">AVERAGE(I43:I52)</f>
+        <v>2.7591840000000003</v>
       </c>
       <c r="K57" s="2"/>
       <c r="M57" s="2"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="2">
+        <f>_xlfn.STDEV.P(B43:B52)</f>
+        <v>9.9474631418057582E-3</v>
+      </c>
+      <c r="C58" s="2">
+        <f t="shared" ref="C58:M58" si="33">_xlfn.STDEV.P(C43:C52)</f>
+        <v>8.5449813137914027E-3</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" si="33"/>
+        <v>8.7371763997300678E-3</v>
+      </c>
+      <c r="E58" s="2">
+        <f t="shared" si="33"/>
+        <v>1.2187285400777332E-2</v>
+      </c>
+      <c r="G58" s="2">
+        <f t="shared" ref="G58:M58" si="34">_xlfn.STDEV.P(G43:G52)</f>
+        <v>1.4176627474826281E-2</v>
+      </c>
+      <c r="I58" s="2">
+        <f t="shared" ref="I58:M58" si="35">_xlfn.STDEV.P(I43:I52)</f>
+        <v>1.3378365520496135E-2</v>
+      </c>
+      <c r="K58" s="2"/>
+      <c r="M58" s="2"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>